<commit_message>
Auto commit: 2025-04-15 16:54:42
</commit_message>
<xml_diff>
--- a/Pythonowe Analizy/Excels/statistics_summary.xlsx
+++ b/Pythonowe Analizy/Excels/statistics_summary.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majlo/Desktop/Analizy Portfelowe i Inwestycyjne/Pythonowe Analizy/Excels/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F032CC97-9B86-1140-81BC-BC917B541F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="20900" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_Stats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -61,8 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +131,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +183,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -203,6 +217,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,9 +252,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,14 +428,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,174 +454,174 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.001680318533359123</v>
+        <v>1.680318533359123E-3</v>
       </c>
       <c r="C2">
-        <v>0.0004384598829056899</v>
+        <v>4.3845988290568989E-4</v>
       </c>
       <c r="D2">
-        <v>0.0003944750435901531</v>
+        <v>3.9447504359015311E-4</v>
       </c>
       <c r="E2">
-        <v>0.001667883041054071</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>1.6678830410540709E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.01212013816237958</v>
+        <v>1.2120138162379579E-2</v>
       </c>
       <c r="C3">
-        <v>0.008768799401304136</v>
+        <v>8.7687994013041365E-3</v>
       </c>
       <c r="D3">
-        <v>0.009682087242455971</v>
+        <v>9.6820872424559709E-3</v>
       </c>
       <c r="E3">
-        <v>0.02611597828671097</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>2.6115978286710969E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0001468977490751698</v>
+        <v>1.4689774907516981E-4</v>
       </c>
       <c r="C4">
-        <v>7.689184294031178E-05</v>
+        <v>7.6891842940311783E-5</v>
       </c>
       <c r="D4">
-        <v>9.374281337052866E-05</v>
+        <v>9.3742813370528656E-5</v>
       </c>
       <c r="E4">
-        <v>0.000682044321871959</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>6.8204432187195902E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.5919154978946869</v>
+        <v>0.59191549789468689</v>
       </c>
       <c r="C5">
         <v>-0.1105287580669717</v>
       </c>
       <c r="D5">
-        <v>-0.2056027566836937</v>
+        <v>-0.20560275668369371</v>
       </c>
       <c r="E5">
         <v>0.365842159998503</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>2.118751886055371</v>
+        <v>2.1187518860553709</v>
       </c>
       <c r="C6">
-        <v>1.68037627633386</v>
+        <v>1.6803762763338601</v>
       </c>
       <c r="D6">
-        <v>0.8234479389156926</v>
+        <v>0.82344793891569257</v>
       </c>
       <c r="E6">
-        <v>0.7480267400653826</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.74802674006538261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.001109812330482972</v>
+        <v>-1.1098123304829721E-3</v>
       </c>
       <c r="C7">
-        <v>-0.0004135553347224116</v>
+        <v>-4.1355533472241159E-4</v>
       </c>
       <c r="D7">
-        <v>0.003096265303855309</v>
+        <v>3.0962653038553089E-3</v>
       </c>
       <c r="E7">
-        <v>-0.0003663843479409588</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>-3.6638434794095879E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.01891708907556748</v>
+        <v>-1.8917089075567481E-2</v>
       </c>
       <c r="C8">
-        <v>-0.01369610376757453</v>
+        <v>-1.3696103767574529E-2</v>
       </c>
       <c r="D8">
-        <v>-0.01474104122860803</v>
+        <v>-1.474104122860803E-2</v>
       </c>
       <c r="E8">
-        <v>-0.03972025992795002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-3.9720259927950023E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-0.02454973474837821</v>
+        <v>-2.454973474837821E-2</v>
       </c>
       <c r="C9">
-        <v>-0.02080370111784467</v>
+        <v>-2.0803701117844669E-2</v>
       </c>
       <c r="D9">
-        <v>-0.02440551022792792</v>
+        <v>-2.4405510227927921E-2</v>
       </c>
       <c r="E9">
-        <v>-0.05328350757289443</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>-5.3283507572894427E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>-0.02199167942991705</v>
+        <v>-2.199167942991705E-2</v>
       </c>
       <c r="C10">
-        <v>-0.01860719318697671</v>
+        <v>-1.8607193186976709E-2</v>
       </c>
       <c r="D10">
-        <v>-0.0212880502679782</v>
+        <v>-2.1288050267978201E-2</v>
       </c>
       <c r="E10">
-        <v>-0.04921899791036756</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-4.921899791036756E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>-0.02655910682087396</v>
+        <v>-2.6559106820873962E-2</v>
       </c>
       <c r="C11">
-        <v>-0.02810749015291655</v>
+        <v>-2.810749015291655E-2</v>
       </c>
       <c r="D11">
-        <v>-0.02971962558205153</v>
+        <v>-2.9719625582051531E-2</v>
       </c>
       <c r="E11">
-        <v>-0.05807735089774701</v>
+        <v>-5.8077350897747008E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>